<commit_message>
A few correction on contextual menus
</commit_message>
<xml_diff>
--- a/TestsAndDemos/Etk.Demo.Shops.UI.Excel/Etk.Demo.Shops.UI.Excel.xlsx
+++ b/TestsAndDemos/Etk.Demo.Shops.UI.Excel/Etk.Demo.Shops.UI.Excel.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Etk-git\TestsAndDemos\Etk.Demo.Shops.UI.Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15315" windowHeight="7995"/>
   </bookViews>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>{Name}</t>
   </si>
@@ -91,47 +96,62 @@
     <t>{LDC=,,DisplayName:Customer.Id}</t>
   </si>
   <si>
+    <t>&lt;Template Name='ShopMain' BindingWith='ShopViewModel'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='ShopMain'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Link To='ShopMain' With='ShopsToDisplay'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='ShopExpand'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Link To='ShopExpand'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Header/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='ShopExpand' BindingWith='ShopViewModel' HeaderAsExpander='SC'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='CustomersMain' BindingWith='CustomerViewModel' /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='CustomersMain'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Link To='CustomersMain' With='Customers'/&gt;</t>
+  </si>
+  <si>
+    <t>{{{Customer.Forename} {Customer.Surname}}}</t>
+  </si>
+  <si>
     <t>&lt;Template Name='Main' BindingWith='ShopsViewModel'/&gt;</t>
   </si>
   <si>
-    <t>&lt;Template Name='ShopMain' BindingWith='ShopViewModel'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='ShopMain'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Link To='ShopMain' With='ShopsToDisplay'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='ShopExpand'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Link To='ShopExpand'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Header/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='ShopExpand' BindingWith='ShopViewModel' HeaderAsExpander='SC'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='CustomersMain' BindingWith='CustomerViewModel' /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='CustomersMain'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Link To='CustomersMain' With='Customers'/&gt;</t>
+    <t>&lt;Template Name='Main' BindingWith='ShopViewModel' /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='Customers' BindingWith='CustomerViewModel' ContextMenu='A26'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ContextualMenu Name='CustomerContextMenu'&gt;
+ &lt;MenuItem Caption='Yo !' FaceId='1089' Action='SheetShops,Etk.Demo.Shops.UI.Excel,DisplayName'/&gt;
+  &lt;MenuItem Caption='Yo Yo !!' FaceId='1090' Action='SheetShops,Etk.Demo.Shops.UI.Excel,DisplayName'/&gt;
+&lt;/ContextualMenu&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -342,19 +362,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,13 +494,13 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -503,14 +523,20 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="102">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -618,11 +644,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -664,7 +698,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,9 +730,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -730,6 +765,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -905,12 +941,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -920,15 +956,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -958,12 +997,12 @@
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="J5" s="3"/>
@@ -1010,8 +1049,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="6"/>
@@ -1062,12 +1100,12 @@
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="J12" s="3"/>
@@ -1121,20 +1159,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="81.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="94.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
@@ -1159,7 +1197,7 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1172,12 +1210,12 @@
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
@@ -1251,7 +1289,7 @@
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="17.25" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1264,12 +1302,12 @@
       <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
@@ -1338,10 +1376,117 @@
       <c r="F16"/>
       <c r="G16"/>
     </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="A26" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="16"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="19"/>
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="19"/>
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="19"/>
+      <c r="B29" s="16"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="19"/>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="16"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="19"/>
+      <c r="B34" s="16"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="19"/>
+      <c r="B35" s="16"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="19"/>
+      <c r="B36" s="16"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="19"/>
+      <c r="B37" s="16"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="19"/>
+      <c r="B38" s="16"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A26:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1349,14 +1494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="53.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
@@ -1371,19 +1516,19 @@
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1">
       <c r="A4" s="6" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1">
       <c r="A6" s="10" t="s">
@@ -1405,7 +1550,7 @@
     <row r="7" spans="1:10" s="6" customFormat="1">
       <c r="A7" s="10"/>
       <c r="B7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>1</v>
@@ -1417,25 +1562,25 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="16" t="s">
+    <row r="13" spans="1:10" s="6" customFormat="1">
+      <c r="A13" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="6" customFormat="1">
+      <c r="A14" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="6" customFormat="1">
-      <c r="A13" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="6" customFormat="1">
-      <c r="A14" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>11</v>
@@ -1452,30 +1597,30 @@
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="7"/>
-      <c r="C15" s="16" t="s">
-        <v>34</v>
+      <c r="C15" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A18" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="16" customFormat="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A18" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="14" customFormat="1">
       <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" s="16" customFormat="1">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:6" s="14" customFormat="1">
       <c r="A20" s="10" t="s">
         <v>4</v>
       </c>
@@ -1492,7 +1637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="16" customFormat="1">
+    <row r="21" spans="1:6" s="14" customFormat="1">
       <c r="B21" s="13" t="s">
         <v>23</v>
       </c>
@@ -1503,10 +1648,10 @@
         <v>19</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>